<commit_message>
Routine updates.  Started work on playing music
</commit_message>
<xml_diff>
--- a/VNCPhidget22/VNCPhidget22Explorer/Resources/json/ExcelFolderMaps.xlsx
+++ b/VNCPhidget22/VNCPhidget22Explorer/Resources/json/ExcelFolderMaps.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\chrhodes\VNCPhidgets\VNCPhidget22\VNCPhidget22Explorer\Resources\json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D97BB48-EE86-4271-9BC0-BA13BE9A1837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E90C065F-1942-4E8D-B0C1-E88B671E547B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="4940" windowWidth="28800" windowHeight="15450" xr2:uid="{A0B765C7-ACF9-42AE-BEA1-2DAE057747D1}"/>
+    <workbookView xWindow="5280" yWindow="5280" windowWidth="28800" windowHeight="15450" xr2:uid="{A0B765C7-ACF9-42AE-BEA1-2DAE057747D1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="2025.10.09" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="122">
   <si>
     <t>Cummulative Folder Count</t>
   </si>
@@ -175,6 +176,234 @@
   </si>
   <si>
     <t xml:space="preserve"> - VoltageOutputSequenceConfig_1.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - _ReadMe.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - ~$ExcelFolderMaps.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - ExcelFolderMaps.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Hosts.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - DigitalInputSequence_1.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - DigitalOutputSequence_1.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - DigitalOutputSequence_OpenClose.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Initialization.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_MainShow.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Movement Studies.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Test AS Replacement.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Test.json</t>
+  </si>
+  <si>
+    <t>DigitalOutput\</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_DigitalOutputs.json</t>
+  </si>
+  <si>
+    <t>Hands\</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Hands_Gestures.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Hands_Initialize.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Hands_Move.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Hands_MovementCharacteristics.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Hands_MovementCharacteristics_All.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Hands_Routines.json</t>
+  </si>
+  <si>
+    <t>Left Hand\</t>
+  </si>
+  <si>
+    <t>Right Hand\</t>
+  </si>
+  <si>
+    <t>RCServo\</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_RCServo_MovementCharacteristics.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_RCServo_OpenClose.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_RCServo_PP1.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_RCServo_PP2.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_RCServo_PP3.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_RCServo_PP4.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_RCServos.json</t>
+  </si>
+  <si>
+    <t>Skulls\</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Skulls_Consulting.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Skulls_Initialize.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Skulls_MoveAll.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Skulls_MoveAllAxes.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Skulls_MoveAngles.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Skulls_MovementCharacteristics.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Skulls_MovementCharacteristics_All.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Skulls_Routines.json</t>
+  </si>
+  <si>
+    <t>Device\</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_169501_Skull_012.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_99220_Skull_012.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_99220_Skull_456.json</t>
+  </si>
+  <si>
+    <t>Skull\</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Skull_012_LeftRight.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Skull_012_TiltLeftRight.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Skull_012_UpDown.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Skull_012_YesNoMaybe.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Skull_456_LeftRight.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Skull_456_TiltLeftRight.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Skull_456_UpDown.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Skull_456_YesNoMaybe.json</t>
+  </si>
+  <si>
+    <t>Stepper\</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Stepper_MovementCharacteristics.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Stepper_OpenClose.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Performance_Steppers.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - AdvancedServoSequence_Skulls.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - AdvancedServoSequence_Test A+B+C.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - RCServoSequence_99415.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - RCServoSequence_Move.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - RCServoSequence_MovementCharacteristics.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - RCServoSequence_OpenClose.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - RCServoSequence_Hand_Left 1 Initialization.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - RCServoSequence_Hand_Left 1 Move.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - RCServoSequence_Hand_Right 1 Initialization.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - RCServoSequence_Hand_Right 1 Move.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - RCServoSequence_Skull 1 Initialization.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - RCServoSequence_Skull 2 Initialization.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - RCServoSequence_Skull 3 Initialization.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - RCServoSequence_Skull Move.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - StepperSequence_1.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - StepperSequence_MovementCharacteristics.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - StepperSequence_OpenClose.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - VoltageInputSequence_1.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - VoltageOutputSequence_1.json</t>
   </si>
 </sst>
 </file>
@@ -616,10 +845,1755 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2CF2DBA-6229-4FC2-9F4D-F813B168FCDF}">
+  <dimension ref="A2:O88"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="14.1796875" customWidth="1" outlineLevel="2"/>
+    <col min="3" max="3" width="14.08984375" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="8.7265625" outlineLevel="2"/>
+    <col min="5" max="5" width="7.08984375" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="8.36328125" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="8" width="14.1796875" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="14.08984375" customWidth="1" outlineLevel="2"/>
+    <col min="10" max="10" width="8.7265625" outlineLevel="1"/>
+    <col min="11" max="14" width="3.6328125" customWidth="1"/>
+    <col min="15" max="15" width="20.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="8">
+        <v>18</v>
+      </c>
+      <c r="B3" s="8">
+        <v>67</v>
+      </c>
+      <c r="C3" s="8">
+        <v>445452</v>
+      </c>
+      <c r="E3" s="8">
+        <v>4</v>
+      </c>
+      <c r="F3" s="8">
+        <v>20739</v>
+      </c>
+      <c r="G3" s="9">
+        <v>45939.387615740743</v>
+      </c>
+      <c r="H3" s="9">
+        <v>45939.387615740743</v>
+      </c>
+      <c r="I3" s="9">
+        <v>45939.387997685182</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="F4" s="3">
+        <v>58</v>
+      </c>
+      <c r="G4" s="4">
+        <v>45884.436886574076</v>
+      </c>
+      <c r="H4" s="4">
+        <v>45787.641087962962</v>
+      </c>
+      <c r="I4" s="4">
+        <v>45937.556550925925</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="F5" s="3">
+        <v>165</v>
+      </c>
+      <c r="G5" s="4">
+        <v>45939.387615740743</v>
+      </c>
+      <c r="H5" s="4">
+        <v>45939.387615740743</v>
+      </c>
+      <c r="I5" s="4">
+        <v>45939.387615740743</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="F6" s="3">
+        <v>12187</v>
+      </c>
+      <c r="G6" s="4">
+        <v>45744.542604166665</v>
+      </c>
+      <c r="H6" s="4">
+        <v>45744.542800925927</v>
+      </c>
+      <c r="I6" s="4">
+        <v>45939.387615740743</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="F7" s="3">
+        <v>8329</v>
+      </c>
+      <c r="G7" s="4">
+        <v>45725.506284722222</v>
+      </c>
+      <c r="H7" s="4">
+        <v>45893.614571759259</v>
+      </c>
+      <c r="I7" s="4">
+        <v>45899.654756944445</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="6">
+        <v>0</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6">
+        <v>558</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6">
+        <v>558</v>
+      </c>
+      <c r="G8" s="7">
+        <v>45611.380810185183</v>
+      </c>
+      <c r="H8" s="7">
+        <v>45706.683344907404</v>
+      </c>
+      <c r="I8" s="7">
+        <v>45900.382141203707</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="F9" s="3">
+        <v>558</v>
+      </c>
+      <c r="G9" s="4">
+        <v>45611.380810185183</v>
+      </c>
+      <c r="H9" s="4">
+        <v>45706.683344907404</v>
+      </c>
+      <c r="I9" s="4">
+        <v>45900.382141203707</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="6">
+        <v>0</v>
+      </c>
+      <c r="B10" s="6">
+        <v>2</v>
+      </c>
+      <c r="C10" s="6">
+        <v>7578</v>
+      </c>
+      <c r="E10" s="6">
+        <v>2</v>
+      </c>
+      <c r="F10" s="6">
+        <v>7578</v>
+      </c>
+      <c r="G10" s="7">
+        <v>45813.533275462964</v>
+      </c>
+      <c r="H10" s="7">
+        <v>45817.86078703704</v>
+      </c>
+      <c r="I10" s="7">
+        <v>45935.578599537039</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="F11" s="3">
+        <v>6504</v>
+      </c>
+      <c r="G11" s="4">
+        <v>45706.651979166665</v>
+      </c>
+      <c r="H11" s="4">
+        <v>45817.86078703704</v>
+      </c>
+      <c r="I11" s="4">
+        <v>45900.382013888891</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="F12" s="3">
+        <v>1074</v>
+      </c>
+      <c r="G12" s="4">
+        <v>45813.533275462964</v>
+      </c>
+      <c r="H12" s="4">
+        <v>45813.563125000001</v>
+      </c>
+      <c r="I12" s="4">
+        <v>45935.578599537039</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" s="6">
+        <v>9</v>
+      </c>
+      <c r="B13" s="6">
+        <v>41</v>
+      </c>
+      <c r="C13" s="6">
+        <v>316727</v>
+      </c>
+      <c r="E13" s="6">
+        <v>5</v>
+      </c>
+      <c r="F13" s="6">
+        <v>22677</v>
+      </c>
+      <c r="G13" s="7">
+        <v>45937.556377314817</v>
+      </c>
+      <c r="H13" s="7">
+        <v>45937.698587962965</v>
+      </c>
+      <c r="I13" s="7">
+        <v>45939.387997685182</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="F14" s="3">
+        <v>1934</v>
+      </c>
+      <c r="G14" s="4">
+        <v>45937.553564814814</v>
+      </c>
+      <c r="H14" s="4">
+        <v>45937.558425925927</v>
+      </c>
+      <c r="I14" s="4">
+        <v>45937.558425925927</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="F15" s="3">
+        <v>6804</v>
+      </c>
+      <c r="G15" s="4">
+        <v>45937.556377314817</v>
+      </c>
+      <c r="H15" s="4">
+        <v>45937.559027777781</v>
+      </c>
+      <c r="I15" s="4">
+        <v>45937.559027777781</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="F16" s="3">
+        <v>2443</v>
+      </c>
+      <c r="G16" s="4">
+        <v>45726.786296296297</v>
+      </c>
+      <c r="H16" s="4">
+        <v>45899.656145833331</v>
+      </c>
+      <c r="I16" s="4">
+        <v>45935.578599537039</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F17" s="3">
+        <v>7082</v>
+      </c>
+      <c r="G17" s="4">
+        <v>45726.483043981483</v>
+      </c>
+      <c r="H17" s="4">
+        <v>45899.656134259261</v>
+      </c>
+      <c r="I17" s="4">
+        <v>45935.408518518518</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F18" s="3">
+        <v>4414</v>
+      </c>
+      <c r="G18" s="4">
+        <v>45743.906481481485</v>
+      </c>
+      <c r="H18" s="4">
+        <v>45899.656134259261</v>
+      </c>
+      <c r="I18" s="4">
+        <v>45935.578599537039</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" s="6">
+        <v>0</v>
+      </c>
+      <c r="B19" s="6">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6">
+        <v>4027</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1</v>
+      </c>
+      <c r="F19" s="6">
+        <v>4027</v>
+      </c>
+      <c r="G19" s="7">
+        <v>45817.650173611109</v>
+      </c>
+      <c r="H19" s="7">
+        <v>45899.656145833331</v>
+      </c>
+      <c r="I19" s="7">
+        <v>45935.578599537039</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F20" s="3">
+        <v>4027</v>
+      </c>
+      <c r="G20" s="4">
+        <v>45817.650173611109</v>
+      </c>
+      <c r="H20" s="4">
+        <v>45899.656145833331</v>
+      </c>
+      <c r="I20" s="4">
+        <v>45935.578599537039</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" s="6">
+        <v>2</v>
+      </c>
+      <c r="B21" s="6">
+        <v>6</v>
+      </c>
+      <c r="C21" s="6">
+        <v>81830</v>
+      </c>
+      <c r="E21" s="6">
+        <v>6</v>
+      </c>
+      <c r="F21" s="6">
+        <v>81830</v>
+      </c>
+      <c r="G21" s="7">
+        <v>45903.364027777781</v>
+      </c>
+      <c r="H21" s="7">
+        <v>45937.690208333333</v>
+      </c>
+      <c r="I21" s="7">
+        <v>45939.387997685182</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F22" s="3">
+        <v>16728</v>
+      </c>
+      <c r="G22" s="4">
+        <v>45903.364027777781</v>
+      </c>
+      <c r="H22" s="4">
+        <v>45934.536319444444</v>
+      </c>
+      <c r="I22" s="4">
+        <v>45935.578599537039</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F23" s="3">
+        <v>15186</v>
+      </c>
+      <c r="G23" s="4">
+        <v>45900.345613425925</v>
+      </c>
+      <c r="H23" s="4">
+        <v>45903.457754629628</v>
+      </c>
+      <c r="I23" s="4">
+        <v>45937.542245370372</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F24" s="3">
+        <v>10924</v>
+      </c>
+      <c r="G24" s="4">
+        <v>45900.398344907408</v>
+      </c>
+      <c r="H24" s="4">
+        <v>45903.47755787037</v>
+      </c>
+      <c r="I24" s="4">
+        <v>45937.696562500001</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F25" s="3">
+        <v>23208</v>
+      </c>
+      <c r="G25" s="4">
+        <v>45900.345613425925</v>
+      </c>
+      <c r="H25" s="4">
+        <v>45903.554131944446</v>
+      </c>
+      <c r="I25" s="4">
+        <v>45935.578599537039</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F26" s="3">
+        <v>5307</v>
+      </c>
+      <c r="G26" s="4">
+        <v>45900.345613425925</v>
+      </c>
+      <c r="H26" s="4">
+        <v>45900.345613425925</v>
+      </c>
+      <c r="I26" s="4">
+        <v>45900.44736111111</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F27" s="3">
+        <v>10477</v>
+      </c>
+      <c r="G27" s="4">
+        <v>45900.345613425925</v>
+      </c>
+      <c r="H27" s="4">
+        <v>45937.690208333333</v>
+      </c>
+      <c r="I27" s="4">
+        <v>45937.690208333333</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28" s="6">
+        <v>0</v>
+      </c>
+      <c r="B28" s="6">
+        <v>0</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0</v>
+      </c>
+      <c r="E28" s="6">
+        <v>0</v>
+      </c>
+      <c r="F28" s="6">
+        <v>0</v>
+      </c>
+      <c r="G28" s="7">
+        <v>45899.649293981478</v>
+      </c>
+      <c r="H28" s="7">
+        <v>45899.649293981478</v>
+      </c>
+      <c r="I28" s="7">
+        <v>45939.387997685182</v>
+      </c>
+      <c r="N28" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A29" s="6">
+        <v>0</v>
+      </c>
+      <c r="B29" s="6">
+        <v>0</v>
+      </c>
+      <c r="C29" s="6">
+        <v>0</v>
+      </c>
+      <c r="E29" s="6">
+        <v>0</v>
+      </c>
+      <c r="F29" s="6">
+        <v>0</v>
+      </c>
+      <c r="G29" s="7">
+        <v>45899.648912037039</v>
+      </c>
+      <c r="H29" s="7">
+        <v>45899.648912037039</v>
+      </c>
+      <c r="I29" s="7">
+        <v>45939.387997685182</v>
+      </c>
+      <c r="N29" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A30" s="6">
+        <v>0</v>
+      </c>
+      <c r="B30" s="6">
+        <v>7</v>
+      </c>
+      <c r="C30" s="6">
+        <v>71010</v>
+      </c>
+      <c r="E30" s="6">
+        <v>7</v>
+      </c>
+      <c r="F30" s="6">
+        <v>71010</v>
+      </c>
+      <c r="G30" s="7">
+        <v>45817.418043981481</v>
+      </c>
+      <c r="H30" s="7">
+        <v>45899.654386574075</v>
+      </c>
+      <c r="I30" s="7">
+        <v>45935.578599537039</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F31" s="3">
+        <v>8379</v>
+      </c>
+      <c r="G31" s="4">
+        <v>45816.705671296295</v>
+      </c>
+      <c r="H31" s="4">
+        <v>45899.654386574075</v>
+      </c>
+      <c r="I31" s="4">
+        <v>45935.578599537039</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F32" s="3">
+        <v>8765</v>
+      </c>
+      <c r="G32" s="4">
+        <v>45816.705671296295</v>
+      </c>
+      <c r="H32" s="4">
+        <v>45899.654386574075</v>
+      </c>
+      <c r="I32" s="4">
+        <v>45935.56212962963</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F33" s="3">
+        <v>17944</v>
+      </c>
+      <c r="G33" s="4">
+        <v>45817.417951388888</v>
+      </c>
+      <c r="H33" s="4">
+        <v>45899.654386574075</v>
+      </c>
+      <c r="I33" s="4">
+        <v>45935.578599537039</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F34" s="3">
+        <v>6414</v>
+      </c>
+      <c r="G34" s="4">
+        <v>45817.417951388888</v>
+      </c>
+      <c r="H34" s="4">
+        <v>45899.654386574075</v>
+      </c>
+      <c r="I34" s="4">
+        <v>45935.578599537039</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F35" s="3">
+        <v>8141</v>
+      </c>
+      <c r="G35" s="4">
+        <v>45817.418043981481</v>
+      </c>
+      <c r="H35" s="4">
+        <v>45899.654386574075</v>
+      </c>
+      <c r="I35" s="4">
+        <v>45935.578599537039</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F36" s="3">
+        <v>8750</v>
+      </c>
+      <c r="G36" s="4">
+        <v>45817.417916666665</v>
+      </c>
+      <c r="H36" s="4">
+        <v>45899.654386574075</v>
+      </c>
+      <c r="I36" s="4">
+        <v>45935.578599537039</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F37" s="3">
+        <v>12617</v>
+      </c>
+      <c r="G37" s="4">
+        <v>45817.417812500003</v>
+      </c>
+      <c r="H37" s="4">
+        <v>45899.654386574075</v>
+      </c>
+      <c r="I37" s="4">
+        <v>45935.578599537039</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A38" s="6">
+        <v>2</v>
+      </c>
+      <c r="B38" s="6">
+        <v>19</v>
+      </c>
+      <c r="C38" s="6">
+        <v>133820</v>
+      </c>
+      <c r="E38" s="6">
+        <v>8</v>
+      </c>
+      <c r="F38" s="6">
+        <v>97597</v>
+      </c>
+      <c r="G38" s="7">
+        <v>45794.861562500002</v>
+      </c>
+      <c r="H38" s="7">
+        <v>45937.698587962965</v>
+      </c>
+      <c r="I38" s="7">
+        <v>45937.698587962965</v>
+      </c>
+      <c r="M38" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F39" s="3">
+        <v>4727</v>
+      </c>
+      <c r="G39" s="4">
+        <v>45794.861562500002</v>
+      </c>
+      <c r="H39" s="4">
+        <v>45899.656145833331</v>
+      </c>
+      <c r="I39" s="4">
+        <v>45937.451261574075</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F40" s="3">
+        <v>7322</v>
+      </c>
+      <c r="G40" s="4">
+        <v>45746.399872685186</v>
+      </c>
+      <c r="H40" s="4">
+        <v>45899.656145833331</v>
+      </c>
+      <c r="I40" s="4">
+        <v>45937.542141203703</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F41" s="3">
+        <v>18628</v>
+      </c>
+      <c r="G41" s="4">
+        <v>45786.524942129632</v>
+      </c>
+      <c r="H41" s="4">
+        <v>45899.656145833331</v>
+      </c>
+      <c r="I41" s="4">
+        <v>45937.451261574075</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F42" s="3">
+        <v>12683</v>
+      </c>
+      <c r="G42" s="4">
+        <v>45786.886064814818</v>
+      </c>
+      <c r="H42" s="4">
+        <v>45899.656145833331</v>
+      </c>
+      <c r="I42" s="4">
+        <v>45937.451261574075</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F43" s="3">
+        <v>11467</v>
+      </c>
+      <c r="G43" s="4">
+        <v>45748.561620370368</v>
+      </c>
+      <c r="H43" s="4">
+        <v>45899.656145833331</v>
+      </c>
+      <c r="I43" s="4">
+        <v>45937.451261574075</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F44" s="3">
+        <v>12944</v>
+      </c>
+      <c r="G44" s="4">
+        <v>45781.44427083333</v>
+      </c>
+      <c r="H44" s="4">
+        <v>45899.656145833331</v>
+      </c>
+      <c r="I44" s="4">
+        <v>45935.578599537039</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F45" s="3">
+        <v>5357</v>
+      </c>
+      <c r="G45" s="4">
+        <v>45790.502835648149</v>
+      </c>
+      <c r="H45" s="4">
+        <v>45899.656145833331</v>
+      </c>
+      <c r="I45" s="4">
+        <v>45899.656145833331</v>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F46" s="3">
+        <v>24469</v>
+      </c>
+      <c r="G46" s="4">
+        <v>45787.390127314815</v>
+      </c>
+      <c r="H46" s="4">
+        <v>45937.698587962965</v>
+      </c>
+      <c r="I46" s="4">
+        <v>45937.698587962965</v>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A47" s="6">
+        <v>0</v>
+      </c>
+      <c r="B47" s="6">
+        <v>3</v>
+      </c>
+      <c r="C47" s="6">
+        <v>9662</v>
+      </c>
+      <c r="E47" s="6">
+        <v>3</v>
+      </c>
+      <c r="F47" s="6">
+        <v>9662</v>
+      </c>
+      <c r="G47" s="7">
+        <v>45790.629965277774</v>
+      </c>
+      <c r="H47" s="7">
+        <v>45935.610173611109</v>
+      </c>
+      <c r="I47" s="7">
+        <v>45937.694687499999</v>
+      </c>
+      <c r="N47" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F48" s="3">
+        <v>2749</v>
+      </c>
+      <c r="G48" s="4">
+        <v>45790.629965277774</v>
+      </c>
+      <c r="H48" s="4">
+        <v>45899.656145833331</v>
+      </c>
+      <c r="I48" s="4">
+        <v>45937.694687499999</v>
+      </c>
+      <c r="O48" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F49" s="3">
+        <v>2731</v>
+      </c>
+      <c r="G49" s="4">
+        <v>45790.629965277774</v>
+      </c>
+      <c r="H49" s="4">
+        <v>45899.656145833331</v>
+      </c>
+      <c r="I49" s="4">
+        <v>45937.451249999998</v>
+      </c>
+      <c r="O49" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F50" s="3">
+        <v>4182</v>
+      </c>
+      <c r="G50" s="4">
+        <v>45790.629965277774</v>
+      </c>
+      <c r="H50" s="4">
+        <v>45935.610173611109</v>
+      </c>
+      <c r="I50" s="4">
+        <v>45937.442465277774</v>
+      </c>
+      <c r="O50" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A51" s="6">
+        <v>0</v>
+      </c>
+      <c r="B51" s="6">
+        <v>8</v>
+      </c>
+      <c r="C51" s="6">
+        <v>26561</v>
+      </c>
+      <c r="E51" s="6">
+        <v>8</v>
+      </c>
+      <c r="F51" s="6">
+        <v>26561</v>
+      </c>
+      <c r="G51" s="7">
+        <v>45790.625011574077</v>
+      </c>
+      <c r="H51" s="7">
+        <v>45935.6171412037</v>
+      </c>
+      <c r="I51" s="7">
+        <v>45937.451261574075</v>
+      </c>
+      <c r="N51" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F52" s="3">
+        <v>3393</v>
+      </c>
+      <c r="G52" s="4">
+        <v>45790.621458333335</v>
+      </c>
+      <c r="H52" s="4">
+        <v>45899.656145833331</v>
+      </c>
+      <c r="I52" s="4">
+        <v>45937.451249999998</v>
+      </c>
+      <c r="O52" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F53" s="3">
+        <v>3372</v>
+      </c>
+      <c r="G53" s="4">
+        <v>45790.62400462963</v>
+      </c>
+      <c r="H53" s="4">
+        <v>45899.656145833331</v>
+      </c>
+      <c r="I53" s="4">
+        <v>45937.451249999998</v>
+      </c>
+      <c r="O53" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F54" s="3">
+        <v>3323</v>
+      </c>
+      <c r="G54" s="4">
+        <v>45790.624699074076</v>
+      </c>
+      <c r="H54" s="4">
+        <v>45899.656145833331</v>
+      </c>
+      <c r="I54" s="4">
+        <v>45937.451249999998</v>
+      </c>
+      <c r="O54" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F55" s="3">
+        <v>3180</v>
+      </c>
+      <c r="G55" s="4">
+        <v>45790.619085648148</v>
+      </c>
+      <c r="H55" s="4">
+        <v>45935.6171412037</v>
+      </c>
+      <c r="I55" s="4">
+        <v>45937.428344907406</v>
+      </c>
+      <c r="O55" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F56" s="3">
+        <v>3397</v>
+      </c>
+      <c r="G56" s="4">
+        <v>45790.622361111113</v>
+      </c>
+      <c r="H56" s="4">
+        <v>45899.656145833331</v>
+      </c>
+      <c r="I56" s="4">
+        <v>45937.451261574075</v>
+      </c>
+      <c r="O56" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F57" s="3">
+        <v>3378</v>
+      </c>
+      <c r="G57" s="4">
+        <v>45790.624247685184</v>
+      </c>
+      <c r="H57" s="4">
+        <v>45899.656145833331</v>
+      </c>
+      <c r="I57" s="4">
+        <v>45937.451249999998</v>
+      </c>
+      <c r="O57" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F58" s="3">
+        <v>3333</v>
+      </c>
+      <c r="G58" s="4">
+        <v>45790.625011574077</v>
+      </c>
+      <c r="H58" s="4">
+        <v>45899.656134259261</v>
+      </c>
+      <c r="I58" s="4">
+        <v>45937.451249999998</v>
+      </c>
+      <c r="O58" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F59" s="3">
+        <v>3185</v>
+      </c>
+      <c r="G59" s="4">
+        <v>45790.61917824074</v>
+      </c>
+      <c r="H59" s="4">
+        <v>45935.6171412037</v>
+      </c>
+      <c r="I59" s="4">
+        <v>45937.428344907406</v>
+      </c>
+      <c r="O59" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A60" s="6">
+        <v>0</v>
+      </c>
+      <c r="B60" s="6">
+        <v>3</v>
+      </c>
+      <c r="C60" s="6">
+        <v>3363</v>
+      </c>
+      <c r="E60" s="6">
+        <v>3</v>
+      </c>
+      <c r="F60" s="6">
+        <v>3363</v>
+      </c>
+      <c r="G60" s="7">
+        <v>45817.650046296294</v>
+      </c>
+      <c r="H60" s="7">
+        <v>45899.656134259261</v>
+      </c>
+      <c r="I60" s="7">
+        <v>45935.578599537039</v>
+      </c>
+      <c r="M60" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F61" s="3">
+        <v>233</v>
+      </c>
+      <c r="G61" s="4">
+        <v>45816.705671296295</v>
+      </c>
+      <c r="H61" s="4">
+        <v>45899.656134259261</v>
+      </c>
+      <c r="I61" s="4">
+        <v>45899.656134259261</v>
+      </c>
+      <c r="N61" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F62" s="3">
+        <v>864</v>
+      </c>
+      <c r="G62" s="4">
+        <v>45816.705671296295</v>
+      </c>
+      <c r="H62" s="4">
+        <v>45899.656134259261</v>
+      </c>
+      <c r="I62" s="4">
+        <v>45935.578599537039</v>
+      </c>
+      <c r="N62" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F63" s="3">
+        <v>2266</v>
+      </c>
+      <c r="G63" s="4">
+        <v>45817.650046296294</v>
+      </c>
+      <c r="H63" s="4">
+        <v>45899.656134259261</v>
+      </c>
+      <c r="I63" s="4">
+        <v>45935.578599537039</v>
+      </c>
+      <c r="N63" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A64" s="6">
+        <v>2</v>
+      </c>
+      <c r="B64" s="6">
+        <v>14</v>
+      </c>
+      <c r="C64" s="6">
+        <v>91587</v>
+      </c>
+      <c r="E64" s="6">
+        <v>6</v>
+      </c>
+      <c r="F64" s="6">
+        <v>61258</v>
+      </c>
+      <c r="G64" s="7">
+        <v>45900.400104166663</v>
+      </c>
+      <c r="H64" s="7">
+        <v>45937.714930555558</v>
+      </c>
+      <c r="I64" s="7">
+        <v>45937.714930555558</v>
+      </c>
+      <c r="L64" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F65" s="3">
+        <v>10753</v>
+      </c>
+      <c r="G65" s="4">
+        <v>45744.861377314817</v>
+      </c>
+      <c r="H65" s="4">
+        <v>45787.640983796293</v>
+      </c>
+      <c r="I65" s="4">
+        <v>45935.571493055555</v>
+      </c>
+      <c r="M65" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F66" s="3">
+        <v>6780</v>
+      </c>
+      <c r="G66" s="4">
+        <v>45744.862291666665</v>
+      </c>
+      <c r="H66" s="4">
+        <v>45787.640983796293</v>
+      </c>
+      <c r="I66" s="4">
+        <v>45899.654756944445</v>
+      </c>
+      <c r="M66" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F67" s="3">
+        <v>23682</v>
+      </c>
+      <c r="G67" s="4">
+        <v>45744.860509259262</v>
+      </c>
+      <c r="H67" s="4">
+        <v>45814.45621527778</v>
+      </c>
+      <c r="I67" s="4">
+        <v>45899.655104166668</v>
+      </c>
+      <c r="M67" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F68" s="3">
+        <v>9867</v>
+      </c>
+      <c r="G68" s="4">
+        <v>45726.54146990741</v>
+      </c>
+      <c r="H68" s="4">
+        <v>45815.510081018518</v>
+      </c>
+      <c r="I68" s="4">
+        <v>45900.374074074076</v>
+      </c>
+      <c r="M68" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F69" s="3">
+        <v>3326</v>
+      </c>
+      <c r="G69" s="4">
+        <v>45726.639837962961</v>
+      </c>
+      <c r="H69" s="4">
+        <v>45815.41715277778</v>
+      </c>
+      <c r="I69" s="4">
+        <v>45900.501655092594</v>
+      </c>
+      <c r="M69" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F70" s="3">
+        <v>6850</v>
+      </c>
+      <c r="G70" s="4">
+        <v>45812.394131944442</v>
+      </c>
+      <c r="H70" s="4">
+        <v>45815.432141203702</v>
+      </c>
+      <c r="I70" s="4">
+        <v>45935.562048611115</v>
+      </c>
+      <c r="M70" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A71" s="6">
+        <v>0</v>
+      </c>
+      <c r="B71" s="6">
+        <v>4</v>
+      </c>
+      <c r="C71" s="6">
+        <v>16885</v>
+      </c>
+      <c r="E71" s="6">
+        <v>4</v>
+      </c>
+      <c r="F71" s="6">
+        <v>16885</v>
+      </c>
+      <c r="G71" s="7">
+        <v>45900.400104166663</v>
+      </c>
+      <c r="H71" s="7">
+        <v>45937.714930555558</v>
+      </c>
+      <c r="I71" s="7">
+        <v>45937.714930555558</v>
+      </c>
+      <c r="M71" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F72" s="3">
+        <v>3822</v>
+      </c>
+      <c r="G72" s="4">
+        <v>45900.345613425925</v>
+      </c>
+      <c r="H72" s="4">
+        <v>45937.711817129632</v>
+      </c>
+      <c r="I72" s="4">
+        <v>45937.711817129632</v>
+      </c>
+      <c r="N72" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F73" s="3">
+        <v>4571</v>
+      </c>
+      <c r="G73" s="4">
+        <v>45900.400104166663</v>
+      </c>
+      <c r="H73" s="4">
+        <v>45934.524097222224</v>
+      </c>
+      <c r="I73" s="4">
+        <v>45937.695300925923</v>
+      </c>
+      <c r="N73" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F74" s="3">
+        <v>3900</v>
+      </c>
+      <c r="G74" s="4">
+        <v>45900.345613425925</v>
+      </c>
+      <c r="H74" s="4">
+        <v>45937.714930555558</v>
+      </c>
+      <c r="I74" s="4">
+        <v>45937.714930555558</v>
+      </c>
+      <c r="N74" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F75" s="3">
+        <v>4592</v>
+      </c>
+      <c r="G75" s="4">
+        <v>45900.400104166663</v>
+      </c>
+      <c r="H75" s="4">
+        <v>45934.524293981478</v>
+      </c>
+      <c r="I75" s="4">
+        <v>45934.567106481481</v>
+      </c>
+      <c r="N75" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A76" s="6">
+        <v>0</v>
+      </c>
+      <c r="B76" s="6">
+        <v>4</v>
+      </c>
+      <c r="C76" s="6">
+        <v>13444</v>
+      </c>
+      <c r="E76" s="6">
+        <v>4</v>
+      </c>
+      <c r="F76" s="6">
+        <v>13444</v>
+      </c>
+      <c r="G76" s="7">
+        <v>45746.572731481479</v>
+      </c>
+      <c r="H76" s="7">
+        <v>45937.473449074074</v>
+      </c>
+      <c r="I76" s="7">
+        <v>45937.473449074074</v>
+      </c>
+      <c r="M76" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F77" s="3">
+        <v>3488</v>
+      </c>
+      <c r="G77" s="4">
+        <v>45746.553182870368</v>
+      </c>
+      <c r="H77" s="4">
+        <v>45937.473449074074</v>
+      </c>
+      <c r="I77" s="4">
+        <v>45937.473449074074</v>
+      </c>
+      <c r="N77" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F78" s="3">
+        <v>3491</v>
+      </c>
+      <c r="G78" s="4">
+        <v>45746.553518518522</v>
+      </c>
+      <c r="H78" s="4">
+        <v>45935.561319444445</v>
+      </c>
+      <c r="I78" s="4">
+        <v>45937.442465277774</v>
+      </c>
+      <c r="N78" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F79" s="3">
+        <v>3540</v>
+      </c>
+      <c r="G79" s="4">
+        <v>45746.553449074076</v>
+      </c>
+      <c r="H79" s="4">
+        <v>45937.473449074074</v>
+      </c>
+      <c r="I79" s="4">
+        <v>45937.473449074074</v>
+      </c>
+      <c r="N79" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F80" s="3">
+        <v>2925</v>
+      </c>
+      <c r="G80" s="4">
+        <v>45746.572731481479</v>
+      </c>
+      <c r="H80" s="4">
+        <v>45935.615590277775</v>
+      </c>
+      <c r="I80" s="4">
+        <v>45937.442465277774</v>
+      </c>
+      <c r="N80" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A81" s="6">
+        <v>0</v>
+      </c>
+      <c r="B81" s="6">
+        <v>3</v>
+      </c>
+      <c r="C81" s="6">
+        <v>7143</v>
+      </c>
+      <c r="E81" s="6">
+        <v>3</v>
+      </c>
+      <c r="F81" s="6">
+        <v>7143</v>
+      </c>
+      <c r="G81" s="7">
+        <v>45813.555555555555</v>
+      </c>
+      <c r="H81" s="7">
+        <v>45899.656527777777</v>
+      </c>
+      <c r="I81" s="7">
+        <v>45900.359282407408</v>
+      </c>
+      <c r="L81" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="F82" s="3">
+        <v>1542</v>
+      </c>
+      <c r="G82" s="4">
+        <v>45725.506284722222</v>
+      </c>
+      <c r="H82" s="4">
+        <v>45813.563125000001</v>
+      </c>
+      <c r="I82" s="4">
+        <v>45900.359247685185</v>
+      </c>
+      <c r="M82" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="F83" s="3">
+        <v>4118</v>
+      </c>
+      <c r="G83" s="4">
+        <v>45813.555555555555</v>
+      </c>
+      <c r="H83" s="4">
+        <v>45899.656527777777</v>
+      </c>
+      <c r="I83" s="4">
+        <v>45899.656527777777</v>
+      </c>
+      <c r="M83" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="F84" s="3">
+        <v>1483</v>
+      </c>
+      <c r="G84" s="4">
+        <v>45813.533310185187</v>
+      </c>
+      <c r="H84" s="4">
+        <v>45813.563125000001</v>
+      </c>
+      <c r="I84" s="4">
+        <v>45900.359282407408</v>
+      </c>
+      <c r="M84" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A85" s="6">
+        <v>0</v>
+      </c>
+      <c r="B85" s="6">
+        <v>1</v>
+      </c>
+      <c r="C85" s="6">
+        <v>558</v>
+      </c>
+      <c r="E85" s="6">
+        <v>1</v>
+      </c>
+      <c r="F85" s="6">
+        <v>558</v>
+      </c>
+      <c r="G85" s="7">
+        <v>45611.380879629629</v>
+      </c>
+      <c r="H85" s="7">
+        <v>45706.68246527778</v>
+      </c>
+      <c r="I85" s="7">
+        <v>45900.359363425923</v>
+      </c>
+      <c r="L85" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="F86" s="3">
+        <v>558</v>
+      </c>
+      <c r="G86" s="4">
+        <v>45611.380879629629</v>
+      </c>
+      <c r="H86" s="4">
+        <v>45706.68246527778</v>
+      </c>
+      <c r="I86" s="4">
+        <v>45900.359363425923</v>
+      </c>
+      <c r="M86" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A87" s="6">
+        <v>0</v>
+      </c>
+      <c r="B87" s="6">
+        <v>1</v>
+      </c>
+      <c r="C87" s="6">
+        <v>562</v>
+      </c>
+      <c r="E87" s="6">
+        <v>1</v>
+      </c>
+      <c r="F87" s="6">
+        <v>562</v>
+      </c>
+      <c r="G87" s="7">
+        <v>45611.383321759262</v>
+      </c>
+      <c r="H87" s="7">
+        <v>45706.642013888886</v>
+      </c>
+      <c r="I87" s="7">
+        <v>45900.359375</v>
+      </c>
+      <c r="L87" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="F88" s="3">
+        <v>562</v>
+      </c>
+      <c r="G88" s="4">
+        <v>45611.383321759262</v>
+      </c>
+      <c r="H88" s="4">
+        <v>45706.642013888886</v>
+      </c>
+      <c r="I88" s="4">
+        <v>45900.359375</v>
+      </c>
+      <c r="M88" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B046EE96-FA31-406B-BA7E-AD118AC44CB6}">
   <dimension ref="A2:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0"/>
+    <sheetView topLeftCell="E1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1417,16 +3391,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64FB39E-9675-4B4E-982A-A690D833AB89}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update to latest 3.3.0 VNCDevelopment Assemblies Update build scripts
</commit_message>
<xml_diff>
--- a/VNCPhidget22/VNCPhidget22Explorer/Resources/json/ExcelFolderMaps.xlsx
+++ b/VNCPhidget22/VNCPhidget22Explorer/Resources/json/ExcelFolderMaps.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{E90C065F-1942-4E8D-B0C1-E88B671E547B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="5280" windowWidth="28800" windowHeight="15450" xr2:uid="{A0B765C7-ACF9-42AE-BEA1-2DAE057747D1}"/>
+    <workbookView xWindow="1100" yWindow="1100" windowWidth="28800" windowHeight="15450" xr2:uid="{A0B765C7-ACF9-42AE-BEA1-2DAE057747D1}"/>
   </bookViews>
   <sheets>
     <sheet name="2025.10.09" sheetId="3" r:id="rId1"/>

</xml_diff>